<commit_message>
added 4omini base results with heuristics; wonderful
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-management-github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AAF15D-3C39-5D4F-9461-DA5CF04FFB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CCDC49-A8DE-F044-83AE-0CBB23D7D215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="5860" windowWidth="38400" windowHeight="21600" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="6360" windowWidth="38400" windowHeight="21100" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="join-no-learning" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="18">
   <si>
     <t>no learning</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>4o</t>
-  </si>
-  <si>
-    <t>4o-vision</t>
   </si>
   <si>
     <t>No Heuristics</t>
@@ -536,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25587A43-803C-A145-92E5-0401065CD429}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -556,12 +553,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
@@ -653,14 +650,20 @@
         <v>0.44477028347996</v>
       </c>
       <c r="E5" s="8">
+        <v>0.17204301075268799</v>
+      </c>
+      <c r="F5" s="8">
         <v>0.38318670576734998</v>
       </c>
-      <c r="F5" s="8">
-        <v>0.17204301075268799</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
+      <c r="G5" s="8">
+        <v>0.81264255457803802</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.17139133268165499</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1.5966112740306199E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
@@ -683,127 +686,107 @@
     </row>
     <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
+      <c r="B7" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="C7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.47768002606712201</v>
+      </c>
+      <c r="E7" s="8">
+        <v>2.4437927663734101E-2</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.49494949494949497</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.61681329423264897</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0.17139133268165499</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.207559465623981</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
-      <c r="B8" s="12" t="s">
-        <v>8</v>
-      </c>
+      <c r="B8" s="12"/>
       <c r="C8" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="8">
-        <v>0.47768002606712201</v>
+        <v>0.51580319322254797</v>
       </c>
       <c r="E8" s="8">
-        <v>2.4437927663734101E-2</v>
+        <v>7.6898012381883304E-2</v>
       </c>
       <c r="F8" s="8">
-        <v>0.49494949494949497</v>
+        <v>0.40729879439556799</v>
       </c>
       <c r="G8" s="8">
-        <v>0.61681329423264897</v>
+        <v>0.51873574454219595</v>
       </c>
       <c r="H8" s="8">
-        <v>0.17139133268165499</v>
+        <v>4.3988269794721403E-2</v>
       </c>
       <c r="I8" s="8">
-        <v>0.207559465623981</v>
+        <v>0.43629846855653298</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" s="8">
-        <v>0.51580319322254797</v>
+        <v>0.51352231997393205</v>
       </c>
       <c r="E9" s="8">
-        <v>7.6898012381883304E-2</v>
+        <v>0.207559465623981</v>
       </c>
       <c r="F9" s="8">
-        <v>0.40729879439556799</v>
+        <v>0.27891821440208497</v>
       </c>
       <c r="G9" s="8">
-        <v>0.51873574454219595</v>
+        <v>0.87976539589442804</v>
       </c>
       <c r="H9" s="8">
-        <v>4.3988269794721403E-2</v>
+        <v>0.119908765070055</v>
       </c>
       <c r="I9" s="8">
-        <v>0.43629846855653298</v>
+        <v>3.25839035516454E-4</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="5" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D10" s="8">
-        <v>0.51352231997393205</v>
+        <v>0.63408276311502099</v>
       </c>
       <c r="E10" s="8">
-        <v>0.27891821440208497</v>
+        <v>3.5190615835777102E-2</v>
       </c>
       <c r="F10" s="8">
-        <v>0.207559465623981</v>
+        <v>0.33072662104920098</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0.63408276311502099</v>
-      </c>
-      <c r="E11" s="8">
-        <v>3.5190615835777102E-2</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0.33072662104920098</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A1:C2"/>
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added 4o baseline, with heuristics, amazing results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-management-github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CCDC49-A8DE-F044-83AE-0CBB23D7D215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B696A3E-ED4F-AB4B-9F84-EDDFC10653A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="6360" windowWidth="38400" windowHeight="21100" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="5860" windowWidth="38400" windowHeight="21600" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="join-no-learning" sheetId="1" r:id="rId1"/>
@@ -536,7 +536,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -675,14 +675,20 @@
         <v>0.49560117302052697</v>
       </c>
       <c r="E6" s="8">
+        <v>0.17986314760508301</v>
+      </c>
+      <c r="F6" s="8">
         <v>0.32453567937438899</v>
       </c>
-      <c r="F6" s="8">
-        <v>0.17986314760508301</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="G6" s="8">
+        <v>0.91397849462365499</v>
+      </c>
+      <c r="H6" s="8">
+        <v>3.4538937764744197E-2</v>
+      </c>
+      <c r="I6" s="8">
+        <v>5.1482567611599798E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
@@ -771,14 +777,20 @@
         <v>0.63408276311502099</v>
       </c>
       <c r="E10" s="8">
+        <v>0.33072662104920098</v>
+      </c>
+      <c r="F10" s="8">
         <v>3.5190615835777102E-2</v>
       </c>
-      <c r="F10" s="8">
-        <v>0.33072662104920098</v>
-      </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+      <c r="G10" s="8">
+        <v>0.92733789507983</v>
+      </c>
+      <c r="H10" s="8">
+        <v>7.1358748778103595E-2</v>
+      </c>
+      <c r="I10" s="8">
+        <v>1.3033561420658099E-3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>